<commit_message>
final changes to models
</commit_message>
<xml_diff>
--- a/tables/bael_analysis_tables_160203.xlsx
+++ b/tables/bael_analysis_tables_160203.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="0" windowWidth="23340" windowHeight="17680" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3380" yWindow="820" windowWidth="23340" windowHeight="17680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="AIC" sheetId="1" r:id="rId1"/>
@@ -1344,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1778,7 +1778,7 @@
         <v>5</v>
       </c>
       <c r="D11">
-        <v>-226.780339658477</v>
+        <v>-226.60613511116901</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1787,13 +1787,13 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>0.37616564160315302</v>
+        <v>0.40029706342872801</v>
       </c>
       <c r="H11">
-        <v>118.598503162572</v>
+        <v>118.512857765375</v>
       </c>
       <c r="I11">
-        <v>0.37616564160315302</v>
+        <v>0.40029706342872801</v>
       </c>
       <c r="K11" s="10" t="str">
         <f t="shared" ref="K11:L15" si="17">B11</f>
@@ -1805,7 +1805,7 @@
       </c>
       <c r="M11" s="11">
         <f t="shared" ref="M11:N15" si="18">ROUND(D11, 2)</f>
-        <v>-226.78</v>
+        <v>-226.61</v>
       </c>
       <c r="N11" s="11">
         <f t="shared" si="18"/>
@@ -1817,15 +1817,15 @@
       </c>
       <c r="P11" s="11">
         <f t="shared" si="19"/>
-        <v>0.376</v>
+        <v>0.4</v>
       </c>
       <c r="Q11" s="11">
         <f t="shared" ref="Q11:R15" si="20">ROUND(H11, 2)</f>
-        <v>118.6</v>
+        <v>118.51</v>
       </c>
       <c r="R11" s="11">
         <f t="shared" si="20"/>
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1839,22 +1839,22 @@
         <v>4</v>
       </c>
       <c r="D12">
-        <v>-226.449966192132</v>
+        <v>-226.29381678498001</v>
       </c>
       <c r="E12">
-        <v>0.33037346634500903</v>
+        <v>0.31231832618911398</v>
       </c>
       <c r="F12">
-        <v>0.84773538898840595</v>
+        <v>0.85542302775902102</v>
       </c>
       <c r="G12">
-        <v>0.31888892650852202</v>
+        <v>0.34242332600124797</v>
       </c>
       <c r="H12">
-        <v>117.362914130549</v>
+        <v>117.285797281379</v>
       </c>
       <c r="I12">
-        <v>0.69505456811167499</v>
+        <v>0.74272038942997598</v>
       </c>
       <c r="K12" s="10" t="str">
         <f t="shared" si="17"/>
@@ -1866,27 +1866,27 @@
       </c>
       <c r="M12" s="11">
         <f t="shared" si="18"/>
-        <v>-226.45</v>
+        <v>-226.29</v>
       </c>
       <c r="N12" s="11">
         <f t="shared" si="18"/>
-        <v>0.33</v>
+        <v>0.31</v>
       </c>
       <c r="O12" s="11">
         <f t="shared" si="19"/>
-        <v>0.84799999999999998</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="P12" s="11">
         <f t="shared" si="19"/>
-        <v>0.31900000000000001</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="Q12" s="11">
         <f t="shared" si="20"/>
-        <v>117.36</v>
+        <v>117.29</v>
       </c>
       <c r="R12" s="11">
         <f t="shared" si="20"/>
-        <v>0.7</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1900,19 +1900,19 @@
         <v>6</v>
       </c>
       <c r="D13">
-        <v>-226.36054619087301</v>
+        <v>-225.722048195772</v>
       </c>
       <c r="E13">
-        <v>0.41979346760339797</v>
+        <v>0.88408691539712003</v>
       </c>
       <c r="F13">
-        <v>0.810667956245818</v>
+        <v>0.64272170364255499</v>
       </c>
       <c r="G13">
-        <v>0.30494543188832501</v>
+        <v>0.25727961057002402</v>
       </c>
       <c r="H13">
-        <v>119.473979389143</v>
+        <v>119.156798745774</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1927,23 +1927,23 @@
       </c>
       <c r="M13" s="11">
         <f t="shared" si="18"/>
-        <v>-226.36</v>
+        <v>-225.72</v>
       </c>
       <c r="N13" s="11">
         <f t="shared" si="18"/>
-        <v>0.42</v>
+        <v>0.88</v>
       </c>
       <c r="O13" s="11">
         <f t="shared" si="19"/>
-        <v>0.81100000000000005</v>
+        <v>0.64300000000000002</v>
       </c>
       <c r="P13" s="11">
         <f t="shared" si="19"/>
-        <v>0.30499999999999999</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="Q13" s="11">
         <f t="shared" si="20"/>
-        <v>119.47</v>
+        <v>119.16</v>
       </c>
       <c r="R13" s="11">
         <f t="shared" si="20"/>
@@ -1961,19 +1961,19 @@
         <v>4</v>
       </c>
       <c r="D14">
-        <v>-13.537492937610301</v>
+        <v>-19.002887980029801</v>
       </c>
       <c r="E14">
-        <v>213.242846720866</v>
+        <v>207.60324713113999</v>
       </c>
       <c r="F14" s="12">
-        <v>4.9534089201199799E-47</v>
+        <v>8.3085965868500602E-46</v>
       </c>
       <c r="G14" s="12">
-        <v>1.86330224455971E-47</v>
+        <v>3.32590681493003E-46</v>
       </c>
       <c r="H14">
-        <v>10.9066775032879</v>
+        <v>13.6403328789038</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1988,11 +1988,11 @@
       </c>
       <c r="M14" s="11">
         <f t="shared" si="18"/>
-        <v>-13.54</v>
+        <v>-19</v>
       </c>
       <c r="N14" s="11">
         <f t="shared" si="18"/>
-        <v>213.24</v>
+        <v>207.6</v>
       </c>
       <c r="O14" s="11">
         <f t="shared" si="19"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="Q14" s="11">
         <f t="shared" si="20"/>
-        <v>10.91</v>
+        <v>13.64</v>
       </c>
       <c r="R14" s="11">
         <f t="shared" si="20"/>
@@ -2022,19 +2022,19 @@
         <v>3</v>
       </c>
       <c r="D15">
-        <v>-7.4448560263490497</v>
+        <v>-13.3275398207001</v>
       </c>
       <c r="E15">
-        <v>219.33548363212699</v>
+        <v>213.27859529046901</v>
       </c>
       <c r="F15" s="12">
-        <v>2.3545335682256701E-48</v>
+        <v>4.8656568672486602E-47</v>
       </c>
       <c r="G15" s="12">
-        <v>8.8569463036776904E-49</v>
+        <v>1.9477081556114701E-47</v>
       </c>
       <c r="H15">
-        <v>6.8046197939964399</v>
+        <v>9.7465285310396794</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -2049,11 +2049,11 @@
       </c>
       <c r="M15" s="11">
         <f t="shared" si="18"/>
-        <v>-7.44</v>
+        <v>-13.33</v>
       </c>
       <c r="N15" s="11">
         <f t="shared" si="18"/>
-        <v>219.34</v>
+        <v>213.28</v>
       </c>
       <c r="O15" s="11">
         <f t="shared" si="19"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="Q15" s="11">
         <f t="shared" si="20"/>
-        <v>6.8</v>
+        <v>9.75</v>
       </c>
       <c r="R15" s="11">
         <f t="shared" si="20"/>
@@ -2087,7 +2087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>